<commit_message>
manuscript revisions, added literature
</commit_message>
<xml_diff>
--- a/BLC_reviewer_comments.xlsx
+++ b/BLC_reviewer_comments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>Comment</t>
   </si>
@@ -247,6 +247,18 @@
   <si>
     <t>Kachru, sreedhar, sharma, Robert Fuchs, Maxwell&amp;Fletcher</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ʌ: 1137, æ: 1196 -- added to manuscipt</t>
+  </si>
+  <si>
+    <t>anyway done that; now changed the line in the introduction too</t>
+  </si>
+  <si>
+    <t>put in cover letter</t>
+  </si>
 </sst>
 </file>
 
@@ -269,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,7 +302,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -327,11 +351,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -640,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -674,7 +713,7 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -687,10 +726,10 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="45" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="15" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -705,8 +744,8 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="45">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="3" t="s">
         <v>45</v>
       </c>
@@ -719,8 +758,8 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
@@ -729,65 +768,67 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="45">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="60">
-      <c r="A7" s="10"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="D7" s="13"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="30">
-      <c r="A8" s="10"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="10"/>
-      <c r="B9" s="8">
+      <c r="A9" s="15"/>
+      <c r="B9" s="7">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="105">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -796,17 +837,17 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="75" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="7" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="60" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="3" t="s">
         <v>49</v>
       </c>
@@ -816,8 +857,8 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
@@ -828,7 +869,7 @@
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -843,7 +884,7 @@
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -855,10 +896,10 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="30">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>3</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -869,8 +910,8 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="30">
-      <c r="A17" s="9"/>
-      <c r="B17" s="8">
+      <c r="A17" s="14"/>
+      <c r="B17" s="7">
         <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -882,8 +923,8 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="45">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8">
+      <c r="A18" s="14"/>
+      <c r="B18" s="7">
         <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -894,13 +935,13 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="45">
-      <c r="A19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="8">
-        <v>3</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="A19" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="7">
+        <v>3</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="3"/>
@@ -908,11 +949,11 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="45">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8">
-        <v>3</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="A20" s="14"/>
+      <c r="B20" s="7">
+        <v>3</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="3"/>
@@ -920,11 +961,11 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="45">
-      <c r="A21" s="9"/>
-      <c r="B21" s="8">
-        <v>3</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="7">
+        <v>3</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="3"/>
@@ -932,11 +973,11 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="45">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8">
-        <v>3</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="7">
+        <v>3</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>60</v>
       </c>
       <c r="D22" s="3"/>
@@ -944,10 +985,10 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="60">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="7">
         <v>2</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -959,8 +1000,8 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="45">
-      <c r="A24" s="9"/>
-      <c r="B24" s="8">
+      <c r="A24" s="14"/>
+      <c r="B24" s="7">
         <v>2</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -972,22 +1013,24 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="30">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="8">
-        <v>3</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="7">
+        <v>3</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="45">
-      <c r="A26" s="9"/>
-      <c r="B26" s="8">
+      <c r="A26" s="14"/>
+      <c r="B26" s="7">
         <v>3</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -998,38 +1041,40 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" ht="45">
-      <c r="A27" s="9"/>
-      <c r="B27" s="8">
-        <v>3</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="A27" s="14"/>
+      <c r="B27" s="7">
+        <v>3</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="45">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8">
-        <v>3</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="A28" s="14"/>
+      <c r="B28" s="7">
+        <v>3</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="4"/>
+      <c r="D28" s="8" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="60">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8">
-        <v>3</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="A29" s="14"/>
+      <c r="B29" s="7">
+        <v>3</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="45">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8">
+      <c r="A30" s="14"/>
+      <c r="B30" s="7">
         <v>2</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -1040,61 +1085,63 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="75">
-      <c r="A31" s="9"/>
-      <c r="B31" s="8">
+      <c r="A31" s="14"/>
+      <c r="B31" s="7">
         <v>2</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8">
+      <c r="A32" s="14"/>
+      <c r="B32" s="7">
         <v>2</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="9"/>
-      <c r="B33" s="8">
+      <c r="A33" s="14"/>
+      <c r="B33" s="7">
         <v>2</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" ht="60">
-      <c r="A34" s="9"/>
-      <c r="B34" s="8">
+      <c r="A34" s="14"/>
+      <c r="B34" s="7">
         <v>2</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" ht="30">
-      <c r="A35" s="9"/>
-      <c r="B35" s="8">
+      <c r="A35" s="14"/>
+      <c r="B35" s="7">
         <v>2</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="4"/>
+      <c r="D35" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="9"/>
-      <c r="B36" s="8">
+      <c r="A36" s="14"/>
+      <c r="B36" s="7">
         <v>2</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="4"/>
@@ -1142,17 +1189,18 @@
       <c r="D43" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="A10:A13"/>
+    <mergeCell ref="D6:D9"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A36"/>
-    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
manuscript revision: major edits, figures
</commit_message>
<xml_diff>
--- a/BLC_reviewer_comments.xlsx
+++ b/BLC_reviewer_comments.xlsx
@@ -191,9 +191,6 @@
     <t xml:space="preserve">for this sample: some measure of proficiency, language use patterns, ages and contexts of acquisition, literacy, ages, education levels, languages of education </t>
   </si>
   <si>
-    <t>[LBQ: https://forms.gle/KWm5QaVrxwPZPZPE6]</t>
-  </si>
-  <si>
     <t>rewrite</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>make more explicit: what was compared to what. In results section begining: define each variable and what measure it is</t>
   </si>
   <si>
-    <t>power analysis</t>
-  </si>
-  <si>
     <t>Discussion section is too short</t>
   </si>
   <si>
@@ -258,6 +252,12 @@
   </si>
   <si>
     <t>send a standaradized test to participants</t>
+  </si>
+  <si>
+    <t>power analysis result figures, write, [remaining simulations]</t>
+  </si>
+  <si>
+    <t>[LBQ: https://forms.gle/KWm5QaVrxwPZPZPE6]   collate info from new survey, see how much is therer. Rest -- see if LBQ gives enough info. Finalize set of participant info available. Compare with Olson. See which IE papers we have cited, some easy info available? Make a list.</t>
   </si>
 </sst>
 </file>
@@ -281,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,12 +308,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF66"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -331,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -366,7 +360,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -679,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -716,51 +713,51 @@
       <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>51</v>
+      <c r="C2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="45" customHeight="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="60">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="3" t="s">
+    <row r="4" spans="1:6" ht="75">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>46</v>
+      <c r="D4" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4"/>
@@ -768,67 +765,67 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="45">
-      <c r="A6" s="15" t="s">
-        <v>52</v>
+      <c r="A6" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="60">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="13"/>
+      <c r="C7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="14"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="30">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="13"/>
+      <c r="C8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="14"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="7">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="105">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="16" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -837,28 +834,28 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="75" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="60" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
@@ -872,11 +869,11 @@
       <c r="B14" s="7">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -896,7 +893,7 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="30">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="7">
@@ -910,7 +907,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="30">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="7">
         <v>3</v>
       </c>
@@ -918,12 +915,12 @@
         <v>19</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="45">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="7">
         <v>3</v>
       </c>
@@ -935,7 +932,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="45">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="7">
@@ -949,7 +946,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="45">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="7">
         <v>3</v>
       </c>
@@ -961,7 +958,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="45">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="7">
         <v>3</v>
       </c>
@@ -973,19 +970,19 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="45">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="7">
         <v>3</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="60">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="7">
@@ -1000,7 +997,7 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="45">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="7">
         <v>2</v>
       </c>
@@ -1013,7 +1010,7 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="30">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="7">
@@ -1023,13 +1020,13 @@
         <v>26</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="45">
-      <c r="A26" s="14"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="7">
         <v>3</v>
       </c>
@@ -1041,7 +1038,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" ht="45">
-      <c r="A27" s="14"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="7">
         <v>3</v>
       </c>
@@ -1051,7 +1048,7 @@
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="45">
-      <c r="A28" s="14"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="7">
         <v>3</v>
       </c>
@@ -1059,11 +1056,11 @@
         <v>29</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="60">
-      <c r="A29" s="14"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="7">
         <v>3</v>
       </c>
@@ -1073,7 +1070,7 @@
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="45">
-      <c r="A30" s="14"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="7">
         <v>2</v>
       </c>
@@ -1081,21 +1078,21 @@
         <v>38</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="75">
-      <c r="A31" s="14"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="7">
         <v>2</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="14"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="7">
         <v>2</v>
       </c>
@@ -1105,7 +1102,7 @@
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="14"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="7">
         <v>2</v>
       </c>
@@ -1115,7 +1112,7 @@
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" ht="60">
-      <c r="A34" s="14"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="7">
         <v>2</v>
       </c>
@@ -1125,19 +1122,19 @@
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" ht="30">
-      <c r="A35" s="14"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="7">
         <v>2</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="11" t="s">
         <v>43</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="14"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="7">
         <v>2</v>
       </c>

</xml_diff>